<commit_message>
Adds Rookie WR Analysis
</commit_message>
<xml_diff>
--- a/data/common/RSP_Rookies.xlsx
+++ b/data/common/RSP_Rookies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/common/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{80AFF0B4-8318-5B46-9F51-C5E54E028385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70761B6A-2211-47F9-BB4F-E96F87F483F7}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{80AFF0B4-8318-5B46-9F51-C5E54E028385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72C7D15C-9B84-4044-8780-6EB1F9234B54}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15460" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1476,8 +1476,24 @@
     <t>Contributor - on the cusp of rotational starter</t>
   </si>
   <si>
+    <t>Better Jalen Hurts at this stage, Malik Wallis as a pospect, Lamar Jackson, Dan Marino</t>
+  </si>
+  <si>
+    <t>Baker Mayfield (High End) – Tua Tagovailoa / Geno Smith (Mid-Range/Stylistic) – Spencer Rattler (Low End/Score Comp)</t>
+  </si>
+  <si>
+    <t>Jake Plummer / J.J. McCarthy (High End / Stylistic) – Drew Lock / Zach Wilson (Low End / Volatility)</t>
+  </si>
+  <si>
+    <t>Official Spectrum: Josh Allen / Andrew Luck (High End / Toolsy Potential) – Tim Tebow / Bryce Petty (Low End / Limited Passer)
+Elaborated Comparison: The "Frankenstein" analogy (Allen + Tebow DNA) producing either Luck (refined) or Howard ("Young Frankenstein" - raw potential) highlights his profile as having high-upside physical tools but significant questions about processing and passing refinement, leading to a wide range of potential outcomes.</t>
+  </si>
+  <si>
+    <t>Official Spectrum: Brock Purdy (High End - efficient system QB) – C.J. Beathard (Low End - career backup/spot starter)</t>
+  </si>
+  <si>
     <t>Strengths:
-Playmaking &amp; Improvisation: Excellent at buying time both inside and outside the pocket, adept at making off-script, against-the-grain throws while moving ("playground creator").
+Playmaking &amp; Improvisation: Excellent at buying time both inside and outside the pocket, adept at making off-script, against-the-grain throws while moving (playground creator).
 Mobility &amp; Pocket Navigation: Possesses excellent movement skills, effectively senses and maneuvers away from pressure (identifies blitzes, climbs, spins, sidesteps), and can create space. Quick enough to escape and reset.
 Arm Talent: Has the required arm strength for the NFL, capable of making most throws, including velocity throws to the boundary, deep pinpoint passes (63-65 yards), and touch throws (moon balls).
 Release &amp; Platform Variety: Quick, whip-like release motion that generates velocity. Can throw effectively from various platforms, including off his back foot (shallow) and on the move. Creative release under pressure on RPOs.
@@ -1490,7 +1506,7 @@
 Footwork Inconsistency: Drop footwork (especially from pistol/shotgun) needs significant tightening; it can be fragmented, slow, bouncy, and lack fluidity, potentially impacting timing in NFL systems. Stance can be too wide, leading to high throws. Cleats sometimes leave the ground during throws.
 Decision-Making Under Pressure/Risk Tolerance: Prone to holding the ball too long, especially in scoring range, leading to avoidable sacks. Takes sizable risks (reversing field, backing away from pressure, high-risk across-body throws) before throwing the ball away. Needs to learn limits and play a more mature game.
 Red Zone Issues: Lapses in awareness of peripheral defenders are more frequent and impactful in the red zone, leading to interceptions or near-interceptions. Can try too hard to make a play in scoring range.
-Accuracy Inconsistencies: While possessing good arm talent, accuracy issues arise, likely linked to footwork. Intermediate mobile accuracy is often just "catchable," not pinpoint. Vertical accuracy towards the boundary under pressure is hit-or-miss. Off-platform accuracy beyond shallow zones is inconsistent.
+Accuracy Inconsistencies: While possessing good arm talent, accuracy issues arise, likely linked to footwork. Intermediate mobile accuracy is often just catchable, not pinpoint. Vertical accuracy towards the boundary under pressure is hit-or-miss. Off-platform accuracy beyond shallow zones is inconsistent.
 Mechanical Refinements: While cautioning against overhauling, the report notes the ball drops low during the draw-back phase, and the upper body mechanics could be tighter.
 Unnecessary Drifting: Has a tendency to drift, particularly to the left, even when unnecessary, which can close off parts of the field and lead to forced throwaways when check-downs might be available.
 Ball Security (Situational): While generally good, not switching the ball to his boundary arm when breaking left makes him vulnerable to fumbles from backside pursuit near the elbow.
@@ -1499,41 +1515,8 @@
 Official Spectrum: Joe Burrow (high-end potential ceiling if technical/mental aspects develop) – Johnny Manziel / Zach Wilson (lower-end outcome/stylistic comparison).
 Elaborated Comparisons:
 Patrick Mahomes: Superficial comparison due to off-script playmaking ability (also compared superficially to Drew Lock and Zach Wilson in the past).
-Johnny Manziel: Closer stylistic comparison due to off-script, creative play style. Ward is seen as having a better off-field mindset. A "refined Manziel" is presented as a potentially compelling outcome.
+Johnny Manziel: Closer stylistic comparison due to off-script, creative play style. Ward is seen as having a better off-field mindset. A refined Manziel is presented as a potentially compelling outcome.
 Joe Burrow: Represents the absolute peak potential if Ward becomes technically sharp and masters processing NFL defenses.</t>
-  </si>
-  <si>
-    <t>Better Jalen Hurts at this stage, Malik Wallis as a pospect, Lamar Jackson, Dan Marino</t>
-  </si>
-  <si>
-    <t>Strengths:
-Pocket Presence &amp; Manipulation: Considered the best pocket player in the class by this evaluator. Possesses "quiet feet" (Lamar Jackson comparison) for subtle, efficient movements. Excellent at manipulating LBs and safeties, even late in the play and under duress. Efficient mover (climb, spin, sidestep, flush) without disrupting offensive structure.
-Release Mechanics: Extremely compact and efficient upper-body release ("most compact in this class," compared favorably to Dan Marino). Draws arm straight back, allowing quick delivery even in tight pockets (truncated/three-quarter motion).
-Arm Strength &amp; Velocity: Can deliver throws 40-48 yards to the opposite hash on a line. Capable of pinpoint deep throws (58 yards near-side flat mentioned). Generates significant torque.
-Mobility &amp; Running Ability: Game-breaking speed ("fastest QB in this draft"). Excellent acceleration, curvilinear movement ("like a big-play scat back"), sudden cuts, and ability to weave through the field (mentions 21 mph speed). Presses LOS effectively, bounces outside, transitions downhill quickly, uses spins/hip shifts. Knows how to slide. Considered a better runner than Jalen Hurts (at the same stage) by this evaluator.
-Decision-Making: Generally a good decision-maker, with gaffes more typical of NFL starters than "Hero Ball." Identifies pre-snap pressure and likely coverage holes. Aware of peripheral defenders and uses placement to protect receivers. Aggressive attacking leverage up the seam. Quick processor under pressure, works through reads. Wise in situational football (e.g., two-minute drill).
-Accuracy Under Pressure: Capable of pinpoint accuracy deep (48 yards) with pressure in face. Accurate off-platform in shallow/intermediate ranges, even when hit. Excellent mobile accuracy, including deep pinpoint throws (53 yards back-shoulder mentioned). Understands when to take velocity off throws under pressure.
-Play Fakes &amp; Pump Fakes: Good detail on read fakes. Uses pump fakes effectively to freeze defenders both from pocket and on the move, often paired with eye manipulation.
-Poise &amp; Intangibles: Handles pressure well, waits appropriately before moving. Mature handling of pre-draft process noted. Won academic Heisman. Showed wisdom in handling bad snap near own endzone.
-Durability: No significant injuries noted.
-Weaknesses:
-Lack of Touch: Significant weakness. Needs to develop touch and learn to put more air/arc under passes. Struggles significantly with fades (throws on a line), honey-hole shots (Cover 2), and back-shoulder throws requiring touch, often overshooting these targets.
-Lower Body Mechanics (Situational): While generally good, lower body mechanics need refinement for touch/trajectory throws. Feet aren't always aligned properly after climbing under pressure, causing some vertical throws to sail.
-Ball Security (Situational): Can be loose with the ball when initially carrying it before seeing pursuit. When breaking the pocket, can carry the ball wide or like a triple-option QB, making him susceptible to strips from backside pursuit.
-Awareness of Undercutting Defenders: Does not consistently see shallow flat/boundary defenders sliding to undercut throws (both shallow and deeper crossing routes). Needs more awareness of this ancillary coverage.
-Holding Ball Post-Scramble (Minor): Has occasional lapses holding the ball too long after making the first defender miss and breaking the pocket (noted in black zone). Worth monitoring but not deemed a major issue yet.
-Play Fake Nuance: Fakes are good but could use more nuance/detail to be truly deceptive.
-Acclimation to NFL: Will need time to adjust to NFL playbook size and complexity of defensive schemes/disguises compared to college.
-Player Comparisons:
-Official Spectrum: Jalen Hurts (High End) – Malik Willis (Low End)
-Elaborated Comparisons:
-Jalen Hurts: Strong comparison. The evaluator sees Milroe as potentially a better runner, pocket manager, and game manager than Hurts was coming out, but notes Hurts' work ethic/obsession is a key unknown variable for Milroe.
-Malik Willis: Used more as a prospect archetype comparison – a toolsy, mobile QB needing development, representing what evaluators hoped Willis would be, rather than a direct stylistic comp to Willis' pro performance. Milroe is seen as less of a long-term project than Jordan Love but not as NFL-ready as Lamar Jackson was.
-Lamar Jackson: Compared specifically for his "quiet feet" and subtle pocket movement.
-Dan Marino: Compared favorably regarding the compactness and efficiency of his upper-body release mechanics.</t>
-  </si>
-  <si>
-    <t>Baker Mayfield (High End) – Tua Tagovailoa / Geno Smith (Mid-Range/Stylistic) – Spencer Rattler (Low End/Score Comp)</t>
   </si>
   <si>
     <t>Strengths:
@@ -1544,40 +1527,37 @@
 Technique (Upper Body/Drops): Efficient, compact, over-the-shoulder release with a high release point and good weight transfer. Well-defined and generally well-paced drops (though 3-step needs quicker pacing). Effective sidearm release for RPO/screens. Good play-action fakes (thorough exchange/fakes).
 Scrambling (Evasiveness): Uses stop-start moves effectively to make defenders overrun angles. Strong enough to pull through reaches. Has short-area quickness in traffic.
 Weaknesses:
-Athleticism/Mobility Limits: Not a dynamic mover (compared athletically to Mayfield/Smith, not Allen/Hurts/Jackson). Lacks high-end mobility for designed sprints and can't outrun edge pressure if it gets close late. Re-start quickness after stopping is "not notable." Moves like a "slow Kyler Murray." May enter the league overconfident in athletic limits.
+Athleticism/Mobility Limits: Not a dynamic mover (compared athletically to Mayfield/Smith, not Allen/Hurts/Jackson). Lacks high-end mobility for designed sprints and cant outrun edge pressure if it gets close late. Re-start quickness after stopping is not notable. Moves like a slow Kyler Murray. May enter the league overconfident in athletic limits.
 Decision-Making (Specific Situations): Struggles identifying leverage advantages quickly on deep middle vertical routes. Prone to targeting intermediate routes breaking back to him (boundary) when a defender has leverage over the top, especially from the far hash and critically, in his own red zone (black zone). Needs to mature as a game manager, be more conservative, and minimize risk in these spots.
 Processing Speed (Specific Situations): Not proficient reading sideline-to-sideline quickly. Can be faster identifying reads even on same-side quick concepts (e.g., double slants). Not strong identifying or pulling the trigger on tight windows over flat defenders.
 Holding Ball Too Long: Can hold the ball too long while looking downfield after abandoning the pocket, leading to avoidable sacks (a habit noted in the middle of the field and red zone). Needs to throw the ball away earlier, especially on designed sprints where his mobility is limited.
 Ball Security: Significant lapses when breaking the pocket – ball drops low and is waved around, leading to forced fumbles by pursuit. Also cited as responsible for multiple bad snaps in the red zone.
 Lack of Middle Field Manipulation: Does not demonstrate manipulation of defenders (LBs/safeties) in the middle of the field with eyes or fakes.
-Arm Talent (Adequate, Not Elite): Has the arm for vertical shots, but arm talent isn't seen as a "difference-making" trait. Accuracy deep requires receiver separation/slowing down at 50+ yards. Needs better trajectory (lower) on some deep boundary throws for pinpoint placement.
+Arm Talent (Adequate, Not Elite): Has the arm for vertical shots, but arm talent isnt seen as a difference-making trait. Accuracy deep requires receiver separation/slowing down at 50+ yards. Needs better trajectory (lower) on some deep boundary throws for pinpoint placement.
 Technique (Lower Body/Fakes): Front foot pointing on out-breaking routes needs improvement (can lead to ball placement behind target/strain). Pump fakes lack violence/effectiveness.
-NFL Readiness: Evaluator explicitly states he shouldn't be thrust into starting role immediately and needs a good situation (OL, run game) to potentially succeed early.
+NFL Readiness: Evaluator explicitly states he shouldnt be thrust into starting role immediately and needs a good situation (OL, run game) to potentially succeed early.
 Player Comparisons:
 Official Spectrum: Baker Mayfield (High End) – Tua Tagovailoa / Geno Smith (Mid-Range/Stylistic) – Spencer Rattler (Low End/Score Comp)
 Elaborated Comparisons:
-Geno Smith / Tua Tagovailoa: Represents his "aspiring" passing style – distributor, quick game, anticipation-based.
-Baker Mayfield / Geno Smith: Used as the "archetypical wheelhouse" for his athleticism – not elite runners, needed time to calibrate physical limits in the NFL. Sanders is expected to need similar calibration.
+Geno Smith / Tua Tagovailoa: Represents his aspiring passing style – distributor, quick game, anticipation-based.
+Baker Mayfield / Geno Smith: Used as the archetypical wheelhouse for his athleticism – not elite runners, needed time to calibrate physical limits in the NFL. Sanders is expected to need similar calibration.
 Spencer Rattler: Compared on the Depth of Talent Score, but noted as a different style (Rattler = better athlete, Sanders = better decision-maker).
 (Slow) Kyler Murray: Used to describe his scrambling movement style (unorthodox but lacking elite quickness).</t>
-  </si>
-  <si>
-    <t>Jake Plummer / J.J. McCarthy (High End / Stylistic) – Drew Lock / Zach Wilson (Low End / Volatility)</t>
   </si>
   <si>
     <t>Strengths:
 Short-to-Intermediate Accuracy &amp; Processing: Accuracy is solid-to-good within 25-30 yards. Shows pinpoint accuracy in the middle of the field under 25 yards and can layer throws. Processes well in this range, capable of working through 2-3 reads across the field before pressure arrives or checking down. Stellar shallow opposite-hash accuracy.
 Mobility &amp; Scrambling: Maneuvers well from pressure, effectively climbs the pocket (hitches, running climb), sidesteps, and rolls. A chain-moving runner who can buy time effectively before deciding to run. Can avoid multiple pressure points. Pulls through tackles, shows good bend/weave in traffic, and transitions downhill quickly. Better than just a chain-mover, capable of 15-30 yard gains. Knows how to slide.
 Pressure Handling: Identifies pre-snap pressure (inside/outside) and generally responds effectively to various pressure types, including some multi-player pressures. Will stand and deliver against interior pressure.
-Game Management (Situational): Shows wisdom in the red zone, willing to "eat the ball" and protect field goal position if a scripted play isn't there post-snap. Protects receivers with placement in the short/intermediate range. Throws the ball away appropriately when pinned to the boundary.
+Game Management (Situational): Shows wisdom in the red zone, willing to eat the ball and protect field goal position if a scripted play isnt there post-snap. Protects receivers with placement in the short/intermediate range. Throws the ball away appropriately when pinned to the boundary.
 Mechanics (Baseline): Setup, stance, and release lack significant flaws from a basic perspective. Uses multiple arm angles. Drawback is efficient. Footwork alignment is fundamentally sound when undisturbed.
 Arm Strength: Possesses enough arm strength to deliver velocity throws downfield (mentions 54-yard post).
 Durability: No missed games in the past three seasons after a freshman year meniscus injury.
 Weaknesses:
-Deep Accuracy (Major Issue): Accuracy significantly deteriorates beyond 25-30 yards, becoming "scattershot" (overthrows, underthrows, inaccurate placement). This is the primary concern and key developmental hurdle.
+Deep Accuracy (Major Issue): Accuracy significantly deteriorates beyond 25-30 yards, becoming scattershot (overthrows, underthrows, inaccurate placement). This is the primary concern and key developmental hurdle.
 Accuracy Under Duress (Deep): Requires undisturbed feet and a narrower base for downfield accuracy (30-45 yards). When forced to maneuver, his feet get too wide, exacerbating downfield accuracy issues (catchable at best). Must develop precise climbing footwork. The lack of obvious mechanical flaws makes fixing this harder (compared negatively to Jake Locker).
 Decision-Making (Situational): Can waste energy scrambling for short gains when an earlier checkdown offered similar yardage with less risk. Some game management decisions lack savvy (needs experience). Occasionally makes poor decisions on rolls instead of throwing the ball away (e.g., trying to cut back inside on 3rd and short when too far out).
-Ball Security (Running): Ball can become loose when scrambling if he hasn't fully transitioned to a runner mindset. Doesn't always tuck the ball to his boundary arm, leading to fumbles (including a pivotal one).
+Ball Security (Running): Ball can become loose when scrambling if he hasnt fully transitioned to a runner mindset. Doesnt always tuck the ball to his boundary arm, leading to fumbles (including a pivotal one).
 Technique (Refinements): Footwork pacing can be fragmented on 3-step drops, hurting timing/accuracy vs pressure. 7-step drops can be slow/lack uniformity. Play fakes are adequate but could use more sell. Pump fakes lack violence; appears unconfident with grip on forceful fakes. Takes contact with throwing shoulder sometimes when running. Defaults to right arm carrying ball even when left is advisable.
 Pressure Recognition (Minor): Can be a step late identifying Green Dog blitzes. Has more difficulty evading pressure when two rushers arrive simultaneously.
 NFL Readiness/Ceiling: Seen as a projection requiring development, particularly the vertical passing game. Not advisable to start early; needs a good situation (veteran QB, supportive system/talent). Success heavily depends on work ethic and unlocking deep accuracy. Ideal outcome (develops while playing) considered unlikely.
@@ -1590,32 +1570,52 @@
 Jake Plummer: Listed as a high-end comparison on the spectrum.</t>
   </si>
   <si>
-    <t>Official Spectrum: Josh Allen / Andrew Luck (High End / Toolsy Potential) – Tim Tebow / Bryce Petty (Low End / Limited Passer)
-Elaborated Comparison: The "Frankenstein" analogy (Allen + Tebow DNA) producing either Luck (refined) or Howard ("Young Frankenstein" - raw potential) highlights his profile as having high-upside physical tools but significant questions about processing and passing refinement, leading to a wide range of potential outcomes.</t>
-  </si>
-  <si>
     <t>Strengths:
-Physical Tools &amp; Foundation: Possesses good size (6'4", 236 lbs). Arm strength is an asset, capable of stretching the field vertically. Mobility is a strength; can escape the pocket, turn the corner on linebackers, break tackles, and gain yards as a runner. Has a good foundational technique in drops, play fakes, pump fakes, and release mechanics requiring only minor tweaks.
+Pocket Presence &amp; Manipulation: Considered the best pocket player in the class by this evaluator. Possesses quiet feet (Lamar Jackson comparison) for subtle, efficient movements. Excellent at manipulating LBs and safeties, even late in the play and under duress. Efficient mover (climb, spin, sidestep, flush) without disrupting offensive structure.
+Release Mechanics: Extremely compact and efficient upper-body release (most compact in this class, compared favorably to Dan Marino). Draws arm straight back, allowing quick delivery even in tight pockets (truncated/three-quarter motion).
+Arm Strength &amp; Velocity: Can deliver throws 40-48 yards to the opposite hash on a line. Capable of pinpoint deep throws (58 yards near-side flat mentioned). Generates significant torque.
+Mobility &amp; Running Ability: Game-breaking speed (fastest QB in this draft). Excellent acceleration, curvilinear movement (like a big-play scat back), sudden cuts, and ability to weave through the field (mentions 21 mph speed). Presses LOS effectively, bounces outside, transitions downhill quickly, uses spins/hip shifts. Knows how to slide. Considered a better runner than Jalen Hurts (at the same stage) by this evaluator.
+Decision-Making: Generally a good decision-maker, with gaffes more typical of NFL starters than Hero Ball. Identifies pre-snap pressure and likely coverage holes. Aware of peripheral defenders and uses placement to protect receivers. Aggressive attacking leverage up the seam. Quick processor under pressure, works through reads. Wise in situational football (e.g., two-minute drill).
+Accuracy Under Pressure: Capable of pinpoint accuracy deep (48 yards) with pressure in face. Accurate off-platform in shallow/intermediate ranges, even when hit. Excellent mobile accuracy, including deep pinpoint throws (53 yards back-shoulder mentioned). Understands when to take velocity off throws under pressure.
+Play Fakes &amp; Pump Fakes: Good detail on read fakes. Uses pump fakes effectively to freeze defenders both from pocket and on the move, often paired with eye manipulation.
+Poise &amp; Intangibles: Handles pressure well, waits appropriately before moving. Mature handling of pre-draft process noted. Won academic Heisman. Showed wisdom in handling bad snap near own endzone.
+Durability: No significant injuries noted.
+Weaknesses:
+Lack of Touch: Significant weakness. Needs to develop touch and learn to put more air/arc under passes. Struggles significantly with fades (throws on a line), honey-hole shots (Cover 2), and back-shoulder throws requiring touch, often overshooting these targets.
+Lower Body Mechanics (Situational): While generally good, lower body mechanics need refinement for touch/trajectory throws. Feet arent always aligned properly after climbing under pressure, causing some vertical throws to sail.
+Ball Security (Situational): Can be loose with the ball when initially carrying it before seeing pursuit. When breaking the pocket, can carry the ball wide or like a triple-option QB, making him susceptible to strips from backside pursuit.
+Awareness of Undercutting Defenders: Does not consistently see shallow flat/boundary defenders sliding to undercut throws (both shallow and deeper crossing routes). Needs more awareness of this ancillary coverage.
+Holding Ball Post-Scramble (Minor): Has occasional lapses holding the ball too long after making the first defender miss and breaking the pocket (noted in black zone). Worth monitoring but not deemed a major issue yet.
+Play Fake Nuance: Fakes are good but could use more nuance/detail to be truly deceptive.
+Acclimation to NFL: Will need time to adjust to NFL playbook size and complexity of defensive schemes/disguises compared to college.
+Player Comparisons:
+Official Spectrum: Jalen Hurts (High End) – Malik Willis (Low End)
+Elaborated Comparisons:
+Jalen Hurts: Strong comparison. The evaluator sees Milroe as potentially a better runner, pocket manager, and game manager than Hurts was coming out, but notes Hurts work ethic/obsession is a key unknown variable for Milroe.
+Malik Willis: Used more as a prospect archetype comparison – a toolsy, mobile QB needing development, representing what evaluators hoped Willis would be, rather than a direct stylistic comp to Willis pro performance. Milroe is seen as less of a long-term project than Jordan Love but not as NFL-ready as Lamar Jackson was.
+Lamar Jackson: Compared specifically for his quiet feet and subtle pocket movement.
+Dan Marino: Compared favorably regarding the compactness and efficiency of his upper-body release mechanics.</t>
+  </si>
+  <si>
+    <t>Strengths:
+Physical Tools &amp; Foundation: Possesses good size (64, 236 lbs). Arm strength is an asset, capable of stretching the field vertically. Mobility is a strength; can escape the pocket, turn the corner on linebackers, break tackles, and gain yards as a runner. Has a good foundational technique in drops, play fakes, pump fakes, and release mechanics requiring only minor tweaks.
 Pocket Manipulation &amp; Poise: Generally drops into a balanced stance with good footwork. Can manipulate defenses by opening his frame during drops. Uses eyes effectively to hold underneath defenders (LBs) to open throwing lanes behind them, showing patience. Can freeze blitzers with stop-start moves.
-Arm Talent (Specific Situations): Shows confidence (bordering on arrogance) in his velocity to fit throws into tight windows, particularly opposite hash throws vs. Cover 2. Has the range for 50-55 yard throws to the opposite boundary. Can "toss" the ball effectively to wide-open vertical targets without needing pinpoint placement. Good touch/placement on opposite boundary fades. Pinpoint accuracy under pressure in specific scenarios (off back foot, mobile, opposite hash curl while hit).
+Arm Talent (Specific Situations): Shows confidence (bordering on arrogance) in his velocity to fit throws into tight windows, particularly opposite hash throws vs. Cover 2. Has the range for 50-55 yard throws to the opposite boundary. Can toss the ball effectively to wide-open vertical targets without needing pinpoint placement. Good touch/placement on opposite boundary fades. Pinpoint accuracy under pressure in specific scenarios (off back foot, mobile, opposite hash curl while hit).
 Mobility &amp; Running: Effective scrambler who can extend plays. Earns chain-moving gains as a runner, showing acceleration to get the edge and balance/strength to break tackles. Improved nuance in selling play-action fakes over time.
 Processing (Basic): Can cycle through 1-2 reads and find the check-down in a timely manner. Accounts for peripheral defenders on first reads from a clean pocket. Identifies pre-snap and post-snap pressure (interior, edge, some DB pressure). Feels blindside pressure appropriately after multiple reads.
 Durability: No significant missed time reported over a five-year career.
 Weaknesses:
-Decision-Making &amp; Risk Assessment: Described as a "mixed bag." Confidence borders on arrogance, leading him to attempt throws into windows/leverage situations that may not work in the NFL. Prone to forcing throws against unfavorable leverage, especially on longer drops when a checkdown is available in space.
-Coverage Recognition/Execution: Struggles significantly with recognizing defenders "squatting" over the top of routes or in throwing lanes (particularly on quick screens), leading to interceptions/pick-sixes. Has difficulty seeing/layering throws over underneath zone defenders and dropping linebackers in the intermediate middle field, resulting in incompletions, INTs, and near-INTs. Doesn't consistently see shallow peripheral defenders peeling off to undercut throws.
+Decision-Making &amp; Risk Assessment: Described as a mixed bag. Confidence borders on arrogance, leading him to attempt throws into windows/leverage situations that may not work in the NFL. Prone to forcing throws against unfavorable leverage, especially on longer drops when a checkdown is available in space.
+Coverage Recognition/Execution: Struggles significantly with recognizing defenders squatting over the top of routes or in throwing lanes (particularly on quick screens), leading to interceptions/pick-sixes. Has difficulty seeing/layering throws over underneath zone defenders and dropping linebackers in the intermediate middle field, resulting in incompletions, INTs, and near-INTs. Doesnt consistently see shallow peripheral defenders peeling off to undercut throws.
 Anticipation: Needs to throw intermediate routes with more anticipation; often releases as the receiver exits the break rather than entering it, giving defenders extra time to react.
-Greediness/Forcing Plays: Lapses on deeper drops where he forgoes an open checkdown after his initial reads aren't open, instead opting to force a covered read or scramble into a prohibitive throw. Attempts throws with pressure in his face where he can't step into it, leading to inaccurate passes and turnover risks.
+Greediness/Forcing Plays: Lapses on deeper drops where he forgoes an open checkdown after his initial reads arent open, instead opting to force a covered read or scramble into a prohibitive throw. Attempts throws with pressure in his face where he cant step into it, leading to inaccurate passes and turnover risks.
 Throwing Mechanics (Minor): While the foundation is good, needs more hip activation for additional torque. Shoulder fakes lack sufficient motion. Play fakes could have more consistent sell/bend.
 Ball Security (Minor): Elbow can be loose from his frame when carrying the ball while scrambling.
-Game Management: Doesn't throw the ball away often (though context suggests few opportunities arose in games watched). Needs to slide feet-first more consistently instead of leading with torso/shoulder.
+Game Management: Doesnt throw the ball away often (though context suggests few opportunities arose in games watched). Needs to slide feet-first more consistently instead of leading with torso/shoulder.
 Player Comparisons:
 Official Spectrum: Josh Allen / Andrew Luck (High End / Toolsy Potential) – Tim Tebow / Bryce Petty (Low End / Limited Passer)
-Elaborated Comparison: The "Frankenstein" analogy (Allen + Tebow DNA) producing either Luck (refined) or Howard ("Young Frankenstein" - raw potential) highlights his profile as having high-upside physical tools but significant questions about processing and passing refinement, leading to a wide range of potential outcomes.
-Overall: Howard presents as a physically gifted quarterback with good arm strength and mobility, fitting the mold of players like Josh Allen or Andrew Luck in terms of raw tools. However, significant weaknesses in decision-making, coverage recognition (especially underneath defenders and squatting coverage), anticipation, and occasional forcing of plays limit his current effectiveness and place him closer to the Tebow/Petty end of the spectrum in terms of potential floor if these issues aren't corrected. He's viewed as having potential as a capable backup with upside, but needs significant development in the mental/processing aspects of the game to have a shot at starting.</t>
-  </si>
-  <si>
-    <t>Official Spectrum: Brock Purdy (High End - efficient system QB) – C.J. Beathard (Low End - career backup/spot starter)</t>
+Elaborated Comparison: The Frankenstein analogy (Allen + Tebow DNA) producing either Luck (refined) or Howard (Young Frankenstein - raw potential) highlights his profile as having high-upside physical tools but significant questions about processing and passing refinement, leading to a wide range of potential outcomes.
+Overall: Howard presents as a physically gifted quarterback with good arm strength and mobility, fitting the mold of players like Josh Allen or Andrew Luck in terms of raw tools. However, significant weaknesses in decision-making, coverage recognition (especially underneath defenders and squatting coverage), anticipation, and occasional forcing of plays limit his current effectiveness and place him closer to the Tebow/Petty end of the spectrum in terms of potential floor if these issues arent corrected. Hes viewed as having potential as a capable backup with upside, but needs significant development in the mental/processing aspects of the game to have a shot at starting.</t>
   </si>
   <si>
     <t>Strengths:
@@ -1626,21 +1626,21 @@
 Situational Awareness (Partial): Throws the ball away appropriately against unblocked/fast pressure when initial reads are covered. Shows wise red-zone management when forced out of the pocket. Places ball well for YAC on checkdowns/outlets. Can identify peeling flat defenders on first reads and make safe throws.
 Scrambling/Running: Can avoid pressure and keep eyes downfield. Pulls through reaches. Makes first defender miss in the flat. Quick enough for chain-moving gains and slides appropriately.
 Weaknesses:
-Deep Accuracy (&gt;42 yards): Accuracy significantly diminishes beyond the ~42-yard mark; described as "lacking" or "mostly inaccurate."
+Deep Accuracy (&gt;42 yards): Accuracy significantly diminishes beyond the ~42-yard mark; described as lacking or mostly inaccurate.
 Placement Nuance: While sometimes aware of peripheral coverage, placement needs refinement for complete protection (currently often partial). Boundary fade placement vs. Cover 3 needs improvement (leads receiver towards safety).
-Processing &amp; Patience: Lapses where he isn't patient enough to let coverage declare (e.g., C2 corner peeling off). Accounting for defenders is less accurate on quick checkdowns vs. initial reads. Needs to show ability to manipulate linebackers with eyes (only noted for safeties). Misses underneath defenders (flat LBs) when working through progressions under pressure.
+Processing &amp; Patience: Lapses where he isnt patient enough to let coverage declare (e.g., C2 corner peeling off). Accounting for defenders is less accurate on quick checkdowns vs. initial reads. Needs to show ability to manipulate linebackers with eyes (only noted for safeties). Misses underneath defenders (flat LBs) when working through progressions under pressure.
 Pocket Clock (Situational): Needs to speed up his internal clock when facing heavy zone coverage with limited receiver options to avoid blindside pressure.
 Pre-Snap Recognition: Must improve pre-snap identification of blindside corner blitzes.
 Game Management (Black Zone): Lacks wisdom in his own end zone (black zone), holding onto the ball too long trying for an extra read after already avoiding pressure, instead of throwing it away.
 Ball Security (Breaking Pocket): Ball carriage is lower and looser than ideal when breaking the pocket.
-Durability: Significant injury history is a concern. Missed multiple games across different seasons due to shoulder (x2), oblique injuries, and had abdominal/ankle issues. (Shoulder '22, non-throwing shoulder '23, oblique '24 cost 2 games, abdominal strain '24 ended game, ankle '24 minor).
+Durability: Significant injury history is a concern. Missed multiple games across different seasons due to shoulder (x2), oblique injuries, and had abdominal/ankle issues. (Shoulder 22, non-throwing shoulder 23, oblique 24 cost 2 games, abdominal strain 24 ended game, ankle 24 minor).
 Player Comparisons:
 Official Spectrum: Brock Purdy (High End - efficient system QB) – C.J. Beathard (Low End - career backup/spot starter)
 Elaborated Comparisons:
-Matt Ryan: Used as context to show that Ewers' effective vertical range (up to ~42 yards) is sufficient for NFL success, even if deep accuracy is lacking.
+Matt Ryan: Used as context to show that Ewers effective vertical range (up to ~42 yards) is sufficient for NFL success, even if deep accuracy is lacking.
 Desmond Ridder: Ewers is viewed more favorably due to seeing leverage better, but potentially fitting a similar role (developmental backup given a chance).
-Overall Projection: The profile leans towards Ewers being a high-level backup or journeyman starter ("at best") rather than a franchise player, aligning more with the Beathard outcome unless placed in an excellent situation that accelerates his development.
-Current Date Context (April 11, 2025): As this profile likely reflects analysis from the previous season or offseason, his status entering the upcoming 2025 season (assuming he's still playing college football per the 'Ohio State '25' game tracked) would depend on his development during that time, but this profile represents a snapshot based on the games listed. The durability concerns remain relevant heading into any future season.</t>
+Overall Projection: The profile leans towards Ewers being a high-level backup or journeyman starter (at best) rather than a franchise player, aligning more with the Beathard outcome unless placed in an excellent situation that accelerates his development.
+Current Date Context (April 11, 2025): As this profile likely reflects analysis from the previous season or offseason, his status entering the upcoming 2025 season (assuming hes still playing college football per the Ohio State 25 game tracked) would depend on his development during that time, but this profile represents a snapshot based on the games listed. The durability concerns remain relevant heading into any future season.</t>
   </si>
 </sst>
 </file>
@@ -2019,7 +2019,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2612,7 +2612,7 @@
         <v>222</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
@@ -2687,7 +2687,7 @@
         <v>111</v>
       </c>
       <c r="F23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G23">
         <v>77</v>
@@ -2696,7 +2696,7 @@
         <v>154</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
@@ -2945,7 +2945,7 @@
         <v>131</v>
       </c>
       <c r="F32" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G32">
         <v>76.599999999999994</v>
@@ -2954,7 +2954,7 @@
         <v>154</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
@@ -3496,7 +3496,7 @@
         <v>218</v>
       </c>
       <c r="F51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G51">
         <v>79</v>
@@ -3505,7 +3505,7 @@
         <v>222</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
@@ -3525,7 +3525,7 @@
         <v>62</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G52">
         <v>76.260000000000005</v>
@@ -3534,7 +3534,7 @@
         <v>154</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
@@ -3554,7 +3554,7 @@
         <v>113</v>
       </c>
       <c r="F53" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G53">
         <v>74</v>

</xml_diff>